<commit_message>
Update to have correct waves
</commit_message>
<xml_diff>
--- a/longitudinal/data_processing_elements_longitudinal-AGN.xlsx
+++ b/longitudinal/data_processing_elements_longitudinal-AGN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A0F523-92FD-4DC7-A5FD-C31D8EE355F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBA2DEE-4E5B-4EF9-889D-3E74CFB97EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DE4C7F53-17AD-41A0-BCA9-A2A8E85C7880}"/>
+    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{DE4C7F53-17AD-41A0-BCA9-A2A8E85C7880}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="401">
   <si>
     <t>index</t>
   </si>
@@ -1332,88 +1332,40 @@
     <t>PA based on one question not available for wave 2, we could base it on multiple question, but would not be consistent with other waves</t>
   </si>
   <si>
-    <t>AGN_1</t>
-  </si>
-  <si>
     <t>AGN_2</t>
   </si>
   <si>
-    <t>date_interview1</t>
-  </si>
-  <si>
     <t>format(as.Date(date_interview4, format = "%d-%m-%Y"), "%Y-%m-%d")</t>
   </si>
   <si>
     <t>floor(as.numeric(Age4))</t>
   </si>
   <si>
-    <t>YPAS_walk_freq1</t>
-  </si>
-  <si>
-    <t>YPAS_sitting1</t>
-  </si>
-  <si>
-    <t>marital_status1</t>
-  </si>
-  <si>
-    <t>Age1</t>
-  </si>
-  <si>
-    <t>floor(as.numeric(Age1))</t>
-  </si>
-  <si>
-    <t>format(as.Date(date_interview1, format = "%d-%m-%Y"), "%Y-%m-%d")</t>
-  </si>
-  <si>
-    <t>MMSE_cor_tot_score1</t>
-  </si>
-  <si>
-    <t>round(MMSE_cor_tot_score1)</t>
-  </si>
-  <si>
     <t>round(MMSE_cor_tot_score4)</t>
   </si>
   <si>
-    <t>CESD_tot_score1</t>
-  </si>
-  <si>
-    <t>height1</t>
-  </si>
-  <si>
-    <t>weight1</t>
-  </si>
-  <si>
-    <t>weight1; 
-height1</t>
-  </si>
-  <si>
-    <t>round(weight1 / (height1/100)^2, 2)</t>
-  </si>
-  <si>
-    <t>ifelse(!is.na(weight1), 2, NA)</t>
-  </si>
-  <si>
-    <t>ifelse(!is.na(height1), 2, NA)</t>
-  </si>
-  <si>
-    <t>waist_circumference1_1; 
-waist_circumference1_2; 
-waist_circumference1_3</t>
-  </si>
-  <si>
-    <t>ifelse(!is.na(waist_circumference1_1) | !is.na(waist_circumference1_2) | !is.na(waist_circumference1_3), 2, NA)</t>
-  </si>
-  <si>
-    <t>round(rowMeans(select(., waist_circumference1_1, waist_circumference1_2, waist_circumference1_3), na.rm = TRUE),2)</t>
-  </si>
-  <si>
-    <t>self_rated_health1</t>
-  </si>
-  <si>
-    <t>Depression_dichotomous1</t>
-  </si>
-  <si>
-    <t>level_of_PA_single_question1</t>
+    <t>date_interview2</t>
+  </si>
+  <si>
+    <t>format(as.Date(date_interview2, format = "%d-%m-%Y"), "%Y-%m-%d")</t>
+  </si>
+  <si>
+    <t>Age2</t>
+  </si>
+  <si>
+    <t>floor(as.numeric(Age2))</t>
+  </si>
+  <si>
+    <t>marital_status2</t>
+  </si>
+  <si>
+    <t>YPAS_sitting2</t>
+  </si>
+  <si>
+    <t>YPAS_walk_freq2</t>
+  </si>
+  <si>
+    <t>AGN_4</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1433,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1800,10 +1752,10 @@
   <dimension ref="A1:AD167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="95.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
@@ -2009,7 +1961,7 @@
         <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="K4" t="s">
         <v>380</v>
@@ -2033,7 +1985,7 @@
         <v>55</v>
       </c>
       <c r="W4" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="45" x14ac:dyDescent="0.25">
@@ -2112,7 +2064,7 @@
         <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K6" t="s">
         <v>381</v>
@@ -2139,10 +2091,10 @@
         <v>55</v>
       </c>
       <c r="W6" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" ht="300" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="135" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2215,7 +2167,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="210" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="90" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2381,7 +2333,7 @@
         <v>101</v>
       </c>
       <c r="J13" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K13" t="s">
         <v>382</v>
@@ -2434,7 +2386,7 @@
         <v>111</v>
       </c>
       <c r="J14" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K14" t="s">
         <v>382</v>
@@ -2464,7 +2416,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2525,43 +2477,25 @@
         <v>118</v>
       </c>
       <c r="J16" t="s">
-        <v>404</v>
-      </c>
-      <c r="K16" t="s">
-        <v>120</v>
-      </c>
-      <c r="M16" t="s">
-        <v>121</v>
-      </c>
-      <c r="O16" t="s">
-        <v>73</v>
-      </c>
-      <c r="P16" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>54</v>
-      </c>
-      <c r="R16" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="T16" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U16" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="V16" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="W16" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="X16" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2584,37 +2518,19 @@
         <v>125</v>
       </c>
       <c r="J17" t="s">
-        <v>404</v>
-      </c>
-      <c r="K17" t="s">
-        <v>120</v>
-      </c>
-      <c r="M17" t="s">
-        <v>121</v>
-      </c>
-      <c r="O17" t="s">
-        <v>73</v>
-      </c>
-      <c r="P17" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>54</v>
-      </c>
-      <c r="R17" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="T17" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U17" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="V17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="W17" t="s">
-        <v>409</v>
+        <v>79</v>
       </c>
       <c r="X17" t="s">
         <v>383</v>
@@ -2643,43 +2559,25 @@
         <v>129</v>
       </c>
       <c r="J18" t="s">
-        <v>405</v>
-      </c>
-      <c r="K18" t="s">
-        <v>131</v>
-      </c>
-      <c r="M18" t="s">
-        <v>132</v>
-      </c>
-      <c r="O18" t="s">
-        <v>73</v>
-      </c>
-      <c r="P18" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>54</v>
-      </c>
-      <c r="R18" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="T18" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U18" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="V18" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="W18" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="X18" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2702,43 +2600,25 @@
         <v>125</v>
       </c>
       <c r="J19" t="s">
-        <v>405</v>
-      </c>
-      <c r="K19" t="s">
-        <v>131</v>
-      </c>
-      <c r="M19" t="s">
-        <v>132</v>
-      </c>
-      <c r="O19" t="s">
-        <v>73</v>
-      </c>
-      <c r="P19" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>54</v>
-      </c>
-      <c r="R19" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="T19" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U19" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="V19" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="W19" t="s">
-        <v>408</v>
+        <v>79</v>
       </c>
       <c r="X19" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2761,43 +2641,26 @@
         <v>138</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="K20" t="s">
-        <v>140</v>
-      </c>
-      <c r="M20" t="s">
-        <v>141</v>
-      </c>
-      <c r="O20" t="s">
-        <v>142</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>144</v>
-      </c>
-      <c r="R20" t="s">
-        <v>145</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="P20" s="1"/>
       <c r="T20" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U20" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="V20" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="W20" t="s">
-        <v>407</v>
+        <v>79</v>
       </c>
       <c r="X20" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="330" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2820,46 +2683,27 @@
         <v>118</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="M21" t="s">
-        <v>151</v>
-      </c>
-      <c r="O21" t="s">
-        <v>152</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>154</v>
-      </c>
-      <c r="R21" t="s">
-        <v>155</v>
-      </c>
-      <c r="S21" t="s">
-        <v>156</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="P21" s="1"/>
       <c r="T21" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U21" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="V21" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="W21" t="s">
-        <v>412</v>
+        <v>79</v>
       </c>
       <c r="X21" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="330" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2882,37 +2726,21 @@
         <v>125</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="M22" t="s">
-        <v>151</v>
-      </c>
-      <c r="O22" t="s">
-        <v>152</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>154</v>
-      </c>
-      <c r="R22" t="s">
-        <v>155</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="P22" s="1"/>
       <c r="T22" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U22" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="V22" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="W22" t="s">
-        <v>411</v>
+        <v>79</v>
       </c>
       <c r="X22" t="s">
         <v>383</v>
@@ -3143,7 +2971,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3523,7 +3351,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="120" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3599,7 +3427,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="120" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3713,7 +3541,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="180" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3751,7 +3579,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="135" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3789,7 +3617,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="105" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3865,7 +3693,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="345" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3888,34 +3716,21 @@
         <v>239</v>
       </c>
       <c r="J48" t="s">
-        <v>413</v>
-      </c>
-      <c r="K48" t="s">
-        <v>241</v>
-      </c>
-      <c r="M48" t="s">
-        <v>242</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="P48" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>244</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="O48" s="1"/>
+      <c r="Q48" s="1"/>
       <c r="T48" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U48" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="V48" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="W48" t="s">
-        <v>245</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -4032,7 +3847,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4260,7 +4075,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4283,28 +4098,23 @@
         <v>249</v>
       </c>
       <c r="J58" t="s">
-        <v>414</v>
-      </c>
-      <c r="K58" t="s">
-        <v>274</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>275</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="L58" s="1"/>
       <c r="T58" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U58" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="V58" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="W58" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4324,34 +4134,21 @@
         <v>43</v>
       </c>
       <c r="J59" t="s">
-        <v>403</v>
-      </c>
-      <c r="K59" t="s">
-        <v>279</v>
-      </c>
-      <c r="M59" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="O59" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="P59" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>282</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="M59" s="1"/>
+      <c r="O59" s="1"/>
       <c r="T59" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U59" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="V59" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="W59" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
@@ -4494,7 +4291,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4514,34 +4311,21 @@
         <v>43</v>
       </c>
       <c r="J64" t="s">
-        <v>400</v>
-      </c>
-      <c r="K64" t="s">
-        <v>294</v>
-      </c>
-      <c r="M64" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="O64" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="P64" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>54</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="M64" s="1"/>
+      <c r="O64" s="1"/>
       <c r="T64" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U64" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="V64" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="W64" t="s">
-        <v>401</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
@@ -4655,7 +4439,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:24" ht="285" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4693,7 +4477,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4731,7 +4515,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:24" ht="195" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4769,7 +4553,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:24" ht="195" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4807,7 +4591,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:24" ht="195" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4845,7 +4629,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="330" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4883,7 +4667,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:24" ht="195" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4921,7 +4705,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:24" ht="195" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5020,7 +4804,7 @@
         <v>337</v>
       </c>
       <c r="J77" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="K77" t="s">
         <v>339</v>
@@ -5073,7 +4857,7 @@
         <v>347</v>
       </c>
       <c r="J78" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="K78" t="s">
         <v>386</v>
@@ -5106,7 +4890,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="79" spans="1:24" ht="360" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5223,7 +5007,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5246,34 +5030,22 @@
         <v>249</v>
       </c>
       <c r="J82" t="s">
-        <v>415</v>
-      </c>
-      <c r="K82" t="s">
-        <v>368</v>
-      </c>
-      <c r="M82" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="O82" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="P82" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q82" s="1" t="s">
-        <v>371</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="M82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="Q82" s="1"/>
       <c r="T82" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="U82" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="V82" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="W82" t="s">
-        <v>372</v>
+        <v>79</v>
       </c>
       <c r="X82" t="s">
         <v>388</v>
@@ -5357,7 +5129,7 @@
         <v>1</v>
       </c>
       <c r="B85" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C85" t="s">
         <v>30</v>
@@ -5404,7 +5176,7 @@
         <v>2</v>
       </c>
       <c r="B86" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C86" t="s">
         <v>41</v>
@@ -5439,7 +5211,7 @@
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C87" t="s">
         <v>46</v>
@@ -5481,7 +5253,7 @@
         <v>55</v>
       </c>
       <c r="W87" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="88" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -5489,7 +5261,7 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C88" t="s">
         <v>56</v>
@@ -5542,7 +5314,7 @@
         <v>5</v>
       </c>
       <c r="B89" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C89" t="s">
         <v>66</v>
@@ -5587,15 +5359,15 @@
         <v>55</v>
       </c>
       <c r="W89" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="90" spans="1:24" ht="300" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C90" t="s">
         <v>75</v>
@@ -5633,7 +5405,7 @@
         <v>7</v>
       </c>
       <c r="B91" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C91" t="s">
         <v>81</v>
@@ -5663,12 +5435,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:24" ht="210" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C92" t="s">
         <v>84</v>
@@ -5706,7 +5478,7 @@
         <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C93" t="s">
         <v>88</v>
@@ -5741,7 +5513,7 @@
         <v>10</v>
       </c>
       <c r="B94" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C94" t="s">
         <v>92</v>
@@ -5776,7 +5548,7 @@
         <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C95" t="s">
         <v>95</v>
@@ -5811,7 +5583,7 @@
         <v>12</v>
       </c>
       <c r="B96" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C96" t="s">
         <v>98</v>
@@ -5864,7 +5636,7 @@
         <v>13</v>
       </c>
       <c r="B97" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C97" t="s">
         <v>108</v>
@@ -5912,12 +5684,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>14</v>
       </c>
       <c r="B98" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C98" t="s">
         <v>113</v>
@@ -5955,7 +5727,7 @@
         <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C99" t="s">
         <v>116</v>
@@ -6006,12 +5778,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="120" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C100" t="s">
         <v>123</v>
@@ -6067,7 +5839,7 @@
         <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C101" t="s">
         <v>127</v>
@@ -6118,12 +5890,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="120" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>18</v>
       </c>
       <c r="B102" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C102" t="s">
         <v>133</v>
@@ -6179,7 +5951,7 @@
         <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C103" t="s">
         <v>136</v>
@@ -6235,7 +6007,7 @@
         <v>20</v>
       </c>
       <c r="B104" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C104" t="s">
         <v>147</v>
@@ -6294,7 +6066,7 @@
         <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C105" t="s">
         <v>158</v>
@@ -6350,7 +6122,7 @@
         <v>22</v>
       </c>
       <c r="B106" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C106" t="s">
         <v>162</v>
@@ -6388,7 +6160,7 @@
         <v>23</v>
       </c>
       <c r="B107" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C107" t="s">
         <v>165</v>
@@ -6423,7 +6195,7 @@
         <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C108" t="s">
         <v>167</v>
@@ -6461,7 +6233,7 @@
         <v>25</v>
       </c>
       <c r="B109" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C109" t="s">
         <v>171</v>
@@ -6499,7 +6271,7 @@
         <v>26</v>
       </c>
       <c r="B110" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C110" t="s">
         <v>174</v>
@@ -6537,7 +6309,7 @@
         <v>27</v>
       </c>
       <c r="B111" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C111" t="s">
         <v>177</v>
@@ -6570,12 +6342,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="120" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>28</v>
       </c>
       <c r="B112" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C112" t="s">
         <v>180</v>
@@ -6613,7 +6385,7 @@
         <v>29</v>
       </c>
       <c r="B113" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C113" t="s">
         <v>183</v>
@@ -6651,7 +6423,7 @@
         <v>30</v>
       </c>
       <c r="B114" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C114" t="s">
         <v>186</v>
@@ -6689,7 +6461,7 @@
         <v>31</v>
       </c>
       <c r="B115" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C115" t="s">
         <v>189</v>
@@ -6727,7 +6499,7 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C116" t="s">
         <v>192</v>
@@ -6765,7 +6537,7 @@
         <v>33</v>
       </c>
       <c r="B117" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C117" t="s">
         <v>194</v>
@@ -6803,7 +6575,7 @@
         <v>34</v>
       </c>
       <c r="B118" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C118" t="s">
         <v>196</v>
@@ -6841,7 +6613,7 @@
         <v>35</v>
       </c>
       <c r="B119" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C119" t="s">
         <v>198</v>
@@ -6879,7 +6651,7 @@
         <v>36</v>
       </c>
       <c r="B120" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C120" t="s">
         <v>200</v>
@@ -6917,7 +6689,7 @@
         <v>37</v>
       </c>
       <c r="B121" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C121" t="s">
         <v>203</v>
@@ -6950,12 +6722,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="120" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>38</v>
       </c>
       <c r="B122" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C122" t="s">
         <v>207</v>
@@ -6993,7 +6765,7 @@
         <v>39</v>
       </c>
       <c r="B123" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C123" t="s">
         <v>211</v>
@@ -7026,12 +6798,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="120" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>40</v>
       </c>
       <c r="B124" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C124" t="s">
         <v>214</v>
@@ -7069,7 +6841,7 @@
         <v>41</v>
       </c>
       <c r="B125" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C125" t="s">
         <v>217</v>
@@ -7107,7 +6879,7 @@
         <v>42</v>
       </c>
       <c r="B126" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C126" t="s">
         <v>220</v>
@@ -7140,12 +6912,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="180" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>43</v>
       </c>
       <c r="B127" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C127" t="s">
         <v>224</v>
@@ -7178,12 +6950,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="135" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>44</v>
       </c>
       <c r="B128" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C128" t="s">
         <v>227</v>
@@ -7216,12 +6988,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="105" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>45</v>
       </c>
       <c r="B129" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C129" t="s">
         <v>231</v>
@@ -7259,7 +7031,7 @@
         <v>46</v>
       </c>
       <c r="B130" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C130" t="s">
         <v>234</v>
@@ -7297,7 +7069,7 @@
         <v>47</v>
       </c>
       <c r="B131" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C131" t="s">
         <v>237</v>
@@ -7350,7 +7122,7 @@
         <v>48</v>
       </c>
       <c r="B132" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C132" t="s">
         <v>246</v>
@@ -7388,7 +7160,7 @@
         <v>49</v>
       </c>
       <c r="B133" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C133" t="s">
         <v>250</v>
@@ -7426,7 +7198,7 @@
         <v>50</v>
       </c>
       <c r="B134" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C134" t="s">
         <v>253</v>
@@ -7459,12 +7231,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>51</v>
       </c>
       <c r="B135" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C135" t="s">
         <v>256</v>
@@ -7502,7 +7274,7 @@
         <v>52</v>
       </c>
       <c r="B136" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C136" t="s">
         <v>260</v>
@@ -7540,7 +7312,7 @@
         <v>53</v>
       </c>
       <c r="B137" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C137" t="s">
         <v>262</v>
@@ -7578,7 +7350,7 @@
         <v>54</v>
       </c>
       <c r="B138" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C138" t="s">
         <v>264</v>
@@ -7616,7 +7388,7 @@
         <v>55</v>
       </c>
       <c r="B139" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C139" t="s">
         <v>266</v>
@@ -7654,7 +7426,7 @@
         <v>56</v>
       </c>
       <c r="B140" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C140" t="s">
         <v>268</v>
@@ -7692,7 +7464,7 @@
         <v>57</v>
       </c>
       <c r="B141" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C141" t="s">
         <v>270</v>
@@ -7736,7 +7508,7 @@
         <v>58</v>
       </c>
       <c r="B142" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C142" t="s">
         <v>276</v>
@@ -7786,7 +7558,7 @@
         <v>59</v>
       </c>
       <c r="B143" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C143" t="s">
         <v>283</v>
@@ -7821,7 +7593,7 @@
         <v>60</v>
       </c>
       <c r="B144" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C144" t="s">
         <v>285</v>
@@ -7856,7 +7628,7 @@
         <v>61</v>
       </c>
       <c r="B145" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C145" t="s">
         <v>287</v>
@@ -7891,7 +7663,7 @@
         <v>62</v>
       </c>
       <c r="B146" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C146" t="s">
         <v>289</v>
@@ -7926,7 +7698,7 @@
         <v>63</v>
       </c>
       <c r="B147" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C147" t="s">
         <v>291</v>
@@ -7968,7 +7740,7 @@
         <v>55</v>
       </c>
       <c r="W147" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
     </row>
     <row r="148" spans="1:23" x14ac:dyDescent="0.25">
@@ -7976,7 +7748,7 @@
         <v>64</v>
       </c>
       <c r="B148" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C148" t="s">
         <v>297</v>
@@ -8011,7 +7783,7 @@
         <v>65</v>
       </c>
       <c r="B149" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C149" t="s">
         <v>299</v>
@@ -8055,7 +7827,7 @@
         <v>66</v>
       </c>
       <c r="B150" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C150" t="s">
         <v>305</v>
@@ -8088,12 +7860,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="285" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23" ht="150" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>67</v>
       </c>
       <c r="B151" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C151" t="s">
         <v>308</v>
@@ -8126,12 +7898,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="90" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>68</v>
       </c>
       <c r="B152" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C152" t="s">
         <v>311</v>
@@ -8164,12 +7936,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="195" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>69</v>
       </c>
       <c r="B153" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C153" t="s">
         <v>314</v>
@@ -8202,12 +7974,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="195" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>70</v>
       </c>
       <c r="B154" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C154" t="s">
         <v>317</v>
@@ -8240,12 +8012,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="195" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>71</v>
       </c>
       <c r="B155" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C155" t="s">
         <v>319</v>
@@ -8278,12 +8050,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23" ht="330" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>72</v>
       </c>
       <c r="B156" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C156" t="s">
         <v>321</v>
@@ -8316,12 +8088,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="195" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>73</v>
       </c>
       <c r="B157" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C157" t="s">
         <v>325</v>
@@ -8354,12 +8126,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="195" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>74</v>
       </c>
       <c r="B158" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C158" t="s">
         <v>328</v>
@@ -8397,7 +8169,7 @@
         <v>75</v>
       </c>
       <c r="B159" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C159" t="s">
         <v>331</v>
@@ -8435,7 +8207,7 @@
         <v>76</v>
       </c>
       <c r="B160" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C160" t="s">
         <v>334</v>
@@ -8488,7 +8260,7 @@
         <v>77</v>
       </c>
       <c r="B161" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C161" t="s">
         <v>344</v>
@@ -8539,12 +8311,12 @@
         <v>354</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="360" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" ht="180" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>78</v>
       </c>
       <c r="B162" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C162" t="s">
         <v>355</v>
@@ -8582,7 +8354,7 @@
         <v>79</v>
       </c>
       <c r="B163" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C163" t="s">
         <v>358</v>
@@ -8620,7 +8392,7 @@
         <v>80</v>
       </c>
       <c r="B164" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C164" t="s">
         <v>361</v>
@@ -8658,7 +8430,7 @@
         <v>81</v>
       </c>
       <c r="B165" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C165" t="s">
         <v>364</v>
@@ -8711,7 +8483,7 @@
         <v>82</v>
       </c>
       <c r="B166" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C166" t="s">
         <v>373</v>
@@ -8746,7 +8518,7 @@
         <v>83</v>
       </c>
       <c r="B167" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C167" t="s">
         <v>376</v>

</xml_diff>